<commit_message>
se modifico  el archivo excel
</commit_message>
<xml_diff>
--- a/software developer/proyeccion de gastos 2022.xlsx
+++ b/software developer/proyeccion de gastos 2022.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\software developer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\GIT\software developer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6012AD59-77FF-43D5-8907-D25901D18E9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7532F374-A3CB-4F33-ACFA-27179C459120}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">gastos mensuales </t>
   </si>
@@ -58,12 +57,18 @@
   </si>
   <si>
     <t>3000 estudiantes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prueba </t>
+  </si>
+  <si>
+    <t>repositorio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
@@ -429,11 +434,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5945DDBA-194B-406C-9C3F-2E4A9A263A07}">
-  <dimension ref="D4:M16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D4:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,6 +602,14 @@
         <v>440000</v>
       </c>
     </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
se le agrega otra fila
</commit_message>
<xml_diff>
--- a/software developer/proyeccion de gastos 2022.xlsx
+++ b/software developer/proyeccion de gastos 2022.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">gastos mensuales </t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>repositorio</t>
+  </si>
+  <si>
+    <t>gastos de estudio</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:M18"/>
+  <dimension ref="D4:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,6 +613,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>